<commit_message>
more assemblers and more verilog
</commit_message>
<xml_diff>
--- a/test/toy_assembler/ISA.xlsx
+++ b/test/toy_assembler/ISA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="212">
   <si>
     <t>HI</t>
   </si>
@@ -20,55 +20,22 @@
     <t>LO-NIBBLE</t>
   </si>
   <si>
-    <t>‐0</t>
-  </si>
-  <si>
-    <t>‐1</t>
-  </si>
-  <si>
-    <t>‐2</t>
-  </si>
-  <si>
-    <t>‐3</t>
-  </si>
-  <si>
-    <t>‐4</t>
-  </si>
-  <si>
-    <t>‐5</t>
-  </si>
-  <si>
-    <t>‐6</t>
-  </si>
-  <si>
-    <t>‐7</t>
-  </si>
-  <si>
-    <t>‐8</t>
-  </si>
-  <si>
-    <t>‐9</t>
-  </si>
-  <si>
-    <t>‐A</t>
-  </si>
-  <si>
-    <t>‐B</t>
-  </si>
-  <si>
-    <t>‐C</t>
-  </si>
-  <si>
-    <t>‐D</t>
-  </si>
-  <si>
-    <t>‐E</t>
-  </si>
-  <si>
-    <t>‐F</t>
-  </si>
-  <si>
-    <t>0‐</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
   <si>
     <t>BRK impl</t>
@@ -101,9 +68,6 @@
     <t>ASL abs</t>
   </si>
   <si>
-    <t>1‐</t>
-  </si>
-  <si>
     <t>BPL rel</t>
   </si>
   <si>
@@ -128,9 +92,6 @@
     <t>ASL abs,X</t>
   </si>
   <si>
-    <t>2‐</t>
-  </si>
-  <si>
     <t>JSR abs</t>
   </si>
   <si>
@@ -164,9 +125,6 @@
     <t>ROL abs</t>
   </si>
   <si>
-    <t>3‐</t>
-  </si>
-  <si>
     <t>BMI rel</t>
   </si>
   <si>
@@ -191,9 +149,6 @@
     <t>ROL abs,X</t>
   </si>
   <si>
-    <t>4‐</t>
-  </si>
-  <si>
     <t>RTI impl</t>
   </si>
   <si>
@@ -224,9 +179,6 @@
     <t>LSR abs</t>
   </si>
   <si>
-    <t>5‐</t>
-  </si>
-  <si>
     <t>BVC rel</t>
   </si>
   <si>
@@ -251,9 +203,6 @@
     <t>LSR abs,X</t>
   </si>
   <si>
-    <t>6‐</t>
-  </si>
-  <si>
     <t>RTS impl</t>
   </si>
   <si>
@@ -284,9 +233,6 @@
     <t>ROR abs</t>
   </si>
   <si>
-    <t>7‐</t>
-  </si>
-  <si>
     <t>BVS rel</t>
   </si>
   <si>
@@ -311,9 +257,6 @@
     <t>ROR abs,X</t>
   </si>
   <si>
-    <t>8‐</t>
-  </si>
-  <si>
     <t>STA X,ind</t>
   </si>
   <si>
@@ -341,9 +284,6 @@
     <t>STX abs</t>
   </si>
   <si>
-    <t>9‐</t>
-  </si>
-  <si>
     <t>BCC rel</t>
   </si>
   <si>
@@ -371,9 +311,6 @@
     <t>STA abs,X</t>
   </si>
   <si>
-    <t>A‐</t>
-  </si>
-  <si>
     <t>LDY #</t>
   </si>
   <si>
@@ -410,9 +347,6 @@
     <t>LDX abs</t>
   </si>
   <si>
-    <t>B‐</t>
-  </si>
-  <si>
     <t>BCS rel</t>
   </si>
   <si>
@@ -446,9 +380,6 @@
     <t>LDX abs,Y</t>
   </si>
   <si>
-    <t>C‐</t>
-  </si>
-  <si>
     <t>CPY #</t>
   </si>
   <si>
@@ -482,9 +413,6 @@
     <t>DEC abs</t>
   </si>
   <si>
-    <t>D‐</t>
-  </si>
-  <si>
     <t>BNE rel</t>
   </si>
   <si>
@@ -509,9 +437,6 @@
     <t>DEC abs,X</t>
   </si>
   <si>
-    <t>E‐</t>
-  </si>
-  <si>
     <t>CPX #</t>
   </si>
   <si>
@@ -545,9 +470,6 @@
     <t>INC abs</t>
   </si>
   <si>
-    <t>F‐</t>
-  </si>
-  <si>
     <t>BEQ rel</t>
   </si>
   <si>
@@ -573,9 +495,6 @@
   </si>
   <si>
     <t>Address Modes</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>Accumulator</t>
@@ -1138,901 +1057,901 @@
     </row>
     <row r="2">
       <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>4.0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>5.0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>8.0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>9.0</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="7">
+        <v>0.0</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="I3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="K3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="L3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="M3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="P3" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="Q3" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="I4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="8" t="s">
+      <c r="L4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="Q4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="I5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="M5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q5" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="D6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="I6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="L6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="8" t="s">
+      <c r="P6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="Q6" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="8" t="s">
+      <c r="D7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="I7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="Q5" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="K7" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="M7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="P7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="8" t="s">
+      <c r="Q7" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" s="8" t="s">
+      <c r="D8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="H8" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="Q6" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="I8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="K8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="L8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="P8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="Q8" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="D9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="H9" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="8" t="s">
+      <c r="I9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="K9" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="L9" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Q7" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="M9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="O9" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="P9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="8" t="s">
+      <c r="Q9" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7">
+        <v>7.0</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="8" t="s">
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="L8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="8" t="s">
+      <c r="I10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="K10" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="L10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="P10" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="Q10" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="D11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="8" t="s">
+      <c r="H11" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="I11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="K11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="M9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="8" t="s">
+      <c r="M11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="O11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P11" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="Q9" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="Q11" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="G12" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H12" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="8" t="s">
+      <c r="I12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K12" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="L10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O10" s="8" t="s">
+      <c r="L12" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="M12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="Q10" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q11" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>118</v>
-      </c>
       <c r="P12" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>119</v>
+        <v>2</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>144</v>
+        <v>4</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="L16" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>165</v>
+        <v>6</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>177</v>
+        <v>7</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2055,189 +1974,189 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>187</v>
+        <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="11" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="11" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="11" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="11" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="11" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="11" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="11" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>228</v>
+        <v>201</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>229</v>
+        <v>202</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>230</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>234</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="11" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>236</v>
+        <v>209</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>238</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>